<commit_message>
avec le bon fichier excel
</commit_message>
<xml_diff>
--- a/HAL_in/StatsBySection.xlsx
+++ b/HAL_in/StatsBySection.xlsx
@@ -1360,16 +1360,16 @@
         <v>36</v>
       </c>
       <c r="C30" t="n">
-        <v>5661</v>
+        <v>4849</v>
       </c>
       <c r="D30" t="n">
-        <v>304.3</v>
+        <v>355.7</v>
       </c>
       <c r="E30" t="n">
-        <v>15.1</v>
+        <v>19.1</v>
       </c>
       <c r="F30" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G30" t="n">
         <v>1</v>

</xml_diff>